<commit_message>
Agregar codigo de graficos
</commit_message>
<xml_diff>
--- a/TSM_vs_Rain.xlsx
+++ b/TSM_vs_Rain.xlsx
@@ -9385,7 +9385,7 @@
         <v>22.7293703799834</v>
       </c>
       <c r="D531" t="n">
-        <v>60.75736627</v>
+        <v>53.45</v>
       </c>
       <c r="E531" s="1" t="n">
         <v>42401</v>
@@ -9402,7 +9402,7 @@
         <v>23.2298279432741</v>
       </c>
       <c r="D532" t="n">
-        <v>132.9843656</v>
+        <v>83.25</v>
       </c>
       <c r="E532" s="1" t="n">
         <v>42430</v>
@@ -9419,7 +9419,7 @@
         <v>20.4237854166667</v>
       </c>
       <c r="D533" t="n">
-        <v>19.67172653</v>
+        <v>10.15</v>
       </c>
       <c r="E533" s="1" t="n">
         <v>42461</v>

</xml_diff>